<commit_message>
Enhanced email sending functionality with improved error handling for CRM connectivity issues. Added progress tracking and debug information for each email sent. Updated dashboard and templates for better user experience, including a footer and responsive design adjustments. Refactored code for clarity and maintainability.
</commit_message>
<xml_diff>
--- a/client-side/template.xlsx
+++ b/client-side/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nullbyte00_/Developer/ongoing_proj/pieds/MassMailingScript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nullbyte00_/Developer/ongoing_proj/pieds/MassMailingScript/client-side/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3F0EFB-FECD-6C46-A8B0-6DAD15ED7954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14992AE7-1CF6-7747-96FA-FCF49DE62D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>COMPANY NAME</t>
   </si>
@@ -43,31 +43,13 @@
     <t>TRACKER</t>
   </si>
   <si>
-    <t>Company A</t>
-  </si>
-  <si>
-    <t>POC A</t>
-  </si>
-  <si>
-    <t>DESIGNATION A</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>srijan.sahay2k5@gmail.com</t>
+    <t>test</t>
   </si>
   <si>
-    <t>Company C</t>
-  </si>
-  <si>
-    <t>POC C</t>
-  </si>
-  <si>
-    <t>DESIGNATION C</t>
-  </si>
-  <si>
-    <t>srijan05sahay@gmail.com</t>
+    <t>dronekill1603@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -86,21 +68,25 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,8 +121,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -145,9 +132,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -364,10 +352,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D15" activeCellId="1" sqref="B98 D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -422,37 +410,663 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="E97" s="4"/>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="E100" s="4"/>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="E101" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{2B4774CD-79AE-394D-A6D4-805310BE6230}"/>
+    <hyperlink ref="E3:E101" r:id="rId2" display="dronekill1603@gmail.com" xr:uid="{68C225EF-F65C-6142-BA8D-9DC45A085A39}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>